<commit_message>
Report++ NF-62 xlsx+pdf !
</commit_message>
<xml_diff>
--- a/resources/template/accounting/_supply.xlsx
+++ b/resources/template/accounting/_supply.xlsx
@@ -180,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -243,6 +243,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -251,8 +254,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:BE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -551,7 +554,9 @@
     <col min="7" max="7" width="9.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="0.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="55" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="56" max="57" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="58" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -569,14 +574,14 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
@@ -585,14 +590,14 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="17" t="s">
@@ -672,35 +677,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G16" s="8" t="s">
+    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="27" t="s">
         <v>12</v>
       </c>
+      <c r="G16" s="27"/>
       <c r="H16" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
     </row>
     <row r="20" spans="2:8" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
@@ -724,13 +730,14 @@
       <c r="H22" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C6:H6"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B19:H19"/>
+    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="96" fitToHeight="999" orientation="portrait" r:id="rId1"/>

</xml_diff>